<commit_message>
Update job postings for 2024-12-17
</commit_message>
<xml_diff>
--- a/javascript-jobs-post/12-17-2024_post.xlsx
+++ b/javascript-jobs-post/12-17-2024_post.xlsx
@@ -91,6 +91,9 @@
     <x:t>AssistRx</x:t>
   </x:si>
   <x:si>
+    <x:t>3D</x:t>
+  </x:si>
+  <x:si>
     <x:t>United States</x:t>
   </x:si>
   <x:si>
@@ -106,9 +109,6 @@
     <x:t>Huawei Telekomünikasyon Dış Ticaret Ltd</x:t>
   </x:si>
   <x:si>
-    <x:t>3D</x:t>
-  </x:si>
-  <x:si>
     <x:t>Turkey</x:t>
   </x:si>
   <x:si>
@@ -145,15 +145,15 @@
     <x:t>Software Developer w Angular ( remote )</x:t>
   </x:si>
   <x:si>
+    <x:t>4D</x:t>
+  </x:si>
+  <x:si>
     <x:t>https://javascript.jobs/job/manager-software-engineering-remote-angular-net-1</x:t>
   </x:si>
   <x:si>
     <x:t>Manager, Software Engineering ( Remote ) - Angular / .net</x:t>
   </x:si>
   <x:si>
-    <x:t>4D</x:t>
-  </x:si>
-  <x:si>
     <x:t>https://javascript.jobs/storage/images/company/676078cedeb83.png</x:t>
   </x:si>
   <x:si>
@@ -208,6 +208,9 @@
     <x:t>Zup</x:t>
   </x:si>
   <x:si>
+    <x:t>5D</x:t>
+  </x:si>
+  <x:si>
     <x:t>https://javascript.jobs/storage/images/company/6714ee528e4b1.png</x:t>
   </x:si>
   <x:si>
@@ -223,9 +226,6 @@
     <x:t>https://javascript.jobs/job/senior-react-native-software-engineer-care</x:t>
   </x:si>
   <x:si>
-    <x:t>5D</x:t>
-  </x:si>
-  <x:si>
     <x:t>Brazil</x:t>
   </x:si>
   <x:si>
@@ -304,6 +304,9 @@
     <x:t>CaseWare</x:t>
   </x:si>
   <x:si>
+    <x:t>6D</x:t>
+  </x:si>
+  <x:si>
     <x:t>Colombia</x:t>
   </x:si>
   <x:si>
@@ -319,9 +322,6 @@
     <x:t>Thoughtworks</x:t>
   </x:si>
   <x:si>
-    <x:t>6D</x:t>
-  </x:si>
-  <x:si>
     <x:t>Chile</x:t>
   </x:si>
   <x:si>
@@ -451,6 +451,9 @@
     <x:t>ONE</x:t>
   </x:si>
   <x:si>
+    <x:t>1W</x:t>
+  </x:si>
+  <x:si>
     <x:t>https://javascript.jobs/job/senior-backend-engineer-nodejsawsk8s-infra-engineering-1</x:t>
   </x:si>
   <x:si>
@@ -460,9 +463,6 @@
     <x:t>https://javascript.jobs/job/senior-full-stack-developer-with-react</x:t>
   </x:si>
   <x:si>
-    <x:t>1W</x:t>
-  </x:si>
-  <x:si>
     <x:t>https://javascript.jobs/storage/images/company/675890fa5c9a6.jpeg</x:t>
   </x:si>
   <x:si>
@@ -982,6 +982,9 @@
     <x:t>Bounteous</x:t>
   </x:si>
   <x:si>
+    <x:t>2W</x:t>
+  </x:si>
+  <x:si>
     <x:t>https://javascript.jobs/storage/images/company/6714ee5a696af.png</x:t>
   </x:si>
   <x:si>
@@ -1004,9 +1007,6 @@
   </x:si>
   <x:si>
     <x:t>LastPass</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2W</x:t>
   </x:si>
   <x:si>
     <x:t>https://javascript.jobs/job/software-engineer-nodejs-5</x:t>
@@ -1556,30 +1556,30 @@
         <x:v>24</x:v>
       </x:c>
       <x:c r="F5" s="0" t="s">
-        <x:v>15</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="G5" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>26</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:7">
       <x:c r="A6" s="0" t="s">
-        <x:v>26</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="B6" s="0" t="s">
-        <x:v>27</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="C6" s="0" t="s">
-        <x:v>28</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="D6" s="0" t="s">
         <x:v>10</x:v>
       </x:c>
       <x:c r="E6" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="F6" s="0" t="s">
-        <x:v>30</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="G6" s="0" t="s">
         <x:v>31</x:v>
@@ -1602,10 +1602,10 @@
         <x:v>24</x:v>
       </x:c>
       <x:c r="F7" s="0" t="s">
-        <x:v>30</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="G7" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>26</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:7">
@@ -1625,7 +1625,7 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="F8" s="0" t="s">
-        <x:v>30</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="G8" s="0" t="s">
         <x:v>13</x:v>
@@ -1648,7 +1648,7 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="F9" s="0" t="s">
-        <x:v>30</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="G9" s="0" t="s">
         <x:v>13</x:v>
@@ -1671,7 +1671,7 @@
         <x:v>39</x:v>
       </x:c>
       <x:c r="F10" s="0" t="s">
-        <x:v>30</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="G10" s="0" t="s">
         <x:v>40</x:v>
@@ -1694,10 +1694,10 @@
         <x:v>24</x:v>
       </x:c>
       <x:c r="F11" s="0" t="s">
-        <x:v>30</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="G11" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>26</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:7">
@@ -1705,10 +1705,10 @@
         <x:v>21</x:v>
       </x:c>
       <x:c r="B12" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="C12" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>45</x:v>
       </x:c>
       <x:c r="D12" s="0" t="s">
         <x:v>10</x:v>
@@ -1717,10 +1717,10 @@
         <x:v>24</x:v>
       </x:c>
       <x:c r="F12" s="0" t="s">
-        <x:v>45</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="G12" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>26</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:7">
@@ -1740,7 +1740,7 @@
         <x:v>49</x:v>
       </x:c>
       <x:c r="F13" s="0" t="s">
-        <x:v>45</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="G13" s="0" t="s">
         <x:v>50</x:v>
@@ -1748,7 +1748,7 @@
     </x:row>
     <x:row r="14" spans="1:7">
       <x:c r="A14" s="0" t="s">
-        <x:v>26</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="B14" s="0" t="s">
         <x:v>51</x:v>
@@ -1760,10 +1760,10 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="E14" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="F14" s="0" t="s">
-        <x:v>45</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="G14" s="0" t="s">
         <x:v>31</x:v>
@@ -1786,7 +1786,7 @@
         <x:v>56</x:v>
       </x:c>
       <x:c r="F15" s="0" t="s">
-        <x:v>45</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="G15" s="0" t="s">
         <x:v>57</x:v>
@@ -1809,7 +1809,7 @@
         <x:v>56</x:v>
       </x:c>
       <x:c r="F16" s="0" t="s">
-        <x:v>45</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="G16" s="0" t="s">
         <x:v>57</x:v>
@@ -1832,7 +1832,7 @@
         <x:v>63</x:v>
       </x:c>
       <x:c r="F17" s="0" t="s">
-        <x:v>45</x:v>
+        <x:v>64</x:v>
       </x:c>
       <x:c r="G17" s="0" t="s">
         <x:v>13</x:v>
@@ -1840,22 +1840,22 @@
     </x:row>
     <x:row r="18" spans="1:7">
       <x:c r="A18" s="0" t="s">
+        <x:v>65</x:v>
+      </x:c>
+      <x:c r="B18" s="0" t="s">
+        <x:v>66</x:v>
+      </x:c>
+      <x:c r="C18" s="0" t="s">
+        <x:v>67</x:v>
+      </x:c>
+      <x:c r="D18" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="E18" s="0" t="s">
+        <x:v>68</x:v>
+      </x:c>
+      <x:c r="F18" s="0" t="s">
         <x:v>64</x:v>
-      </x:c>
-      <x:c r="B18" s="0" t="s">
-        <x:v>65</x:v>
-      </x:c>
-      <x:c r="C18" s="0" t="s">
-        <x:v>66</x:v>
-      </x:c>
-      <x:c r="D18" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="E18" s="0" t="s">
-        <x:v>67</x:v>
-      </x:c>
-      <x:c r="F18" s="0" t="s">
-        <x:v>45</x:v>
       </x:c>
       <x:c r="G18" s="0" t="s">
         <x:v>20</x:v>
@@ -1866,7 +1866,7 @@
         <x:v>53</x:v>
       </x:c>
       <x:c r="B19" s="0" t="s">
-        <x:v>68</x:v>
+        <x:v>69</x:v>
       </x:c>
       <x:c r="C19" s="0" t="s">
         <x:v>59</x:v>
@@ -1878,7 +1878,7 @@
         <x:v>56</x:v>
       </x:c>
       <x:c r="F19" s="0" t="s">
-        <x:v>69</x:v>
+        <x:v>64</x:v>
       </x:c>
       <x:c r="G19" s="0" t="s">
         <x:v>70</x:v>
@@ -1901,7 +1901,7 @@
         <x:v>74</x:v>
       </x:c>
       <x:c r="F20" s="0" t="s">
-        <x:v>69</x:v>
+        <x:v>64</x:v>
       </x:c>
       <x:c r="G20" s="0" t="s">
         <x:v>75</x:v>
@@ -1924,7 +1924,7 @@
         <x:v>79</x:v>
       </x:c>
       <x:c r="F21" s="0" t="s">
-        <x:v>69</x:v>
+        <x:v>64</x:v>
       </x:c>
       <x:c r="G21" s="0" t="s">
         <x:v>80</x:v>
@@ -1947,7 +1947,7 @@
         <x:v>84</x:v>
       </x:c>
       <x:c r="F22" s="0" t="s">
-        <x:v>69</x:v>
+        <x:v>64</x:v>
       </x:c>
       <x:c r="G22" s="0" t="s">
         <x:v>13</x:v>
@@ -1970,7 +1970,7 @@
         <x:v>88</x:v>
       </x:c>
       <x:c r="F23" s="0" t="s">
-        <x:v>69</x:v>
+        <x:v>64</x:v>
       </x:c>
       <x:c r="G23" s="0" t="s">
         <x:v>89</x:v>
@@ -1993,7 +1993,7 @@
         <x:v>84</x:v>
       </x:c>
       <x:c r="F24" s="0" t="s">
-        <x:v>69</x:v>
+        <x:v>64</x:v>
       </x:c>
       <x:c r="G24" s="0" t="s">
         <x:v>13</x:v>
@@ -2016,30 +2016,30 @@
         <x:v>95</x:v>
       </x:c>
       <x:c r="F25" s="0" t="s">
-        <x:v>69</x:v>
+        <x:v>96</x:v>
       </x:c>
       <x:c r="G25" s="0" t="s">
-        <x:v>96</x:v>
+        <x:v>97</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:7">
       <x:c r="A26" s="0" t="s">
-        <x:v>97</x:v>
+        <x:v>98</x:v>
       </x:c>
       <x:c r="B26" s="0" t="s">
-        <x:v>98</x:v>
+        <x:v>99</x:v>
       </x:c>
       <x:c r="C26" s="0" t="s">
-        <x:v>99</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="D26" s="0" t="s">
         <x:v>10</x:v>
       </x:c>
       <x:c r="E26" s="0" t="s">
-        <x:v>100</x:v>
+        <x:v>101</x:v>
       </x:c>
       <x:c r="F26" s="0" t="s">
-        <x:v>101</x:v>
+        <x:v>96</x:v>
       </x:c>
       <x:c r="G26" s="0" t="s">
         <x:v>102</x:v>
@@ -2062,7 +2062,7 @@
         <x:v>106</x:v>
       </x:c>
       <x:c r="F27" s="0" t="s">
-        <x:v>101</x:v>
+        <x:v>96</x:v>
       </x:c>
       <x:c r="G27" s="0" t="s">
         <x:v>40</x:v>
@@ -2085,7 +2085,7 @@
         <x:v>110</x:v>
       </x:c>
       <x:c r="F28" s="0" t="s">
-        <x:v>101</x:v>
+        <x:v>96</x:v>
       </x:c>
       <x:c r="G28" s="0" t="s">
         <x:v>111</x:v>
@@ -2108,7 +2108,7 @@
         <x:v>116</x:v>
       </x:c>
       <x:c r="F29" s="0" t="s">
-        <x:v>101</x:v>
+        <x:v>96</x:v>
       </x:c>
       <x:c r="G29" s="0" t="s">
         <x:v>13</x:v>
@@ -2131,7 +2131,7 @@
         <x:v>120</x:v>
       </x:c>
       <x:c r="F30" s="0" t="s">
-        <x:v>101</x:v>
+        <x:v>96</x:v>
       </x:c>
       <x:c r="G30" s="0" t="s">
         <x:v>121</x:v>
@@ -2154,7 +2154,7 @@
         <x:v>125</x:v>
       </x:c>
       <x:c r="F31" s="0" t="s">
-        <x:v>101</x:v>
+        <x:v>96</x:v>
       </x:c>
       <x:c r="G31" s="0" t="s">
         <x:v>126</x:v>
@@ -2177,7 +2177,7 @@
         <x:v>130</x:v>
       </x:c>
       <x:c r="F32" s="0" t="s">
-        <x:v>101</x:v>
+        <x:v>96</x:v>
       </x:c>
       <x:c r="G32" s="0" t="s">
         <x:v>13</x:v>
@@ -2200,7 +2200,7 @@
         <x:v>56</x:v>
       </x:c>
       <x:c r="F33" s="0" t="s">
-        <x:v>101</x:v>
+        <x:v>96</x:v>
       </x:c>
       <x:c r="G33" s="0" t="s">
         <x:v>70</x:v>
@@ -2223,7 +2223,7 @@
         <x:v>135</x:v>
       </x:c>
       <x:c r="F34" s="0" t="s">
-        <x:v>101</x:v>
+        <x:v>96</x:v>
       </x:c>
       <x:c r="G34" s="0" t="s">
         <x:v>136</x:v>
@@ -2246,10 +2246,10 @@
         <x:v>140</x:v>
       </x:c>
       <x:c r="F35" s="0" t="s">
-        <x:v>101</x:v>
+        <x:v>96</x:v>
       </x:c>
       <x:c r="G35" s="0" t="s">
-        <x:v>96</x:v>
+        <x:v>97</x:v>
       </x:c>
     </x:row>
     <x:row r="36" spans="1:7">
@@ -2269,10 +2269,10 @@
         <x:v>144</x:v>
       </x:c>
       <x:c r="F36" s="0" t="s">
-        <x:v>101</x:v>
+        <x:v>145</x:v>
       </x:c>
       <x:c r="G36" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>26</x:v>
       </x:c>
     </x:row>
     <x:row r="37" spans="1:7">
@@ -2280,10 +2280,10 @@
         <x:v>127</x:v>
       </x:c>
       <x:c r="B37" s="0" t="s">
-        <x:v>145</x:v>
+        <x:v>146</x:v>
       </x:c>
       <x:c r="C37" s="0" t="s">
-        <x:v>146</x:v>
+        <x:v>147</x:v>
       </x:c>
       <x:c r="D37" s="0" t="s">
         <x:v>10</x:v>
@@ -2292,7 +2292,7 @@
         <x:v>130</x:v>
       </x:c>
       <x:c r="F37" s="0" t="s">
-        <x:v>101</x:v>
+        <x:v>145</x:v>
       </x:c>
       <x:c r="G37" s="0" t="s">
         <x:v>70</x:v>
@@ -2303,7 +2303,7 @@
         <x:v>117</x:v>
       </x:c>
       <x:c r="B38" s="0" t="s">
-        <x:v>147</x:v>
+        <x:v>148</x:v>
       </x:c>
       <x:c r="C38" s="0" t="s">
         <x:v>119</x:v>
@@ -2315,7 +2315,7 @@
         <x:v>120</x:v>
       </x:c>
       <x:c r="F38" s="0" t="s">
-        <x:v>148</x:v>
+        <x:v>145</x:v>
       </x:c>
       <x:c r="G38" s="0" t="s">
         <x:v>89</x:v>
@@ -2338,7 +2338,7 @@
         <x:v>152</x:v>
       </x:c>
       <x:c r="F39" s="0" t="s">
-        <x:v>148</x:v>
+        <x:v>145</x:v>
       </x:c>
       <x:c r="G39" s="0" t="s">
         <x:v>13</x:v>
@@ -2361,10 +2361,10 @@
         <x:v>156</x:v>
       </x:c>
       <x:c r="F40" s="0" t="s">
-        <x:v>148</x:v>
+        <x:v>145</x:v>
       </x:c>
       <x:c r="G40" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>26</x:v>
       </x:c>
     </x:row>
     <x:row r="41" spans="1:7">
@@ -2384,7 +2384,7 @@
         <x:v>160</x:v>
       </x:c>
       <x:c r="F41" s="0" t="s">
-        <x:v>148</x:v>
+        <x:v>145</x:v>
       </x:c>
       <x:c r="G41" s="0" t="s">
         <x:v>161</x:v>
@@ -2407,10 +2407,10 @@
         <x:v>165</x:v>
       </x:c>
       <x:c r="F42" s="0" t="s">
-        <x:v>148</x:v>
+        <x:v>145</x:v>
       </x:c>
       <x:c r="G42" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>26</x:v>
       </x:c>
     </x:row>
     <x:row r="43" spans="1:7">
@@ -2430,7 +2430,7 @@
         <x:v>120</x:v>
       </x:c>
       <x:c r="F43" s="0" t="s">
-        <x:v>148</x:v>
+        <x:v>145</x:v>
       </x:c>
       <x:c r="G43" s="0" t="s">
         <x:v>126</x:v>
@@ -2453,7 +2453,7 @@
         <x:v>171</x:v>
       </x:c>
       <x:c r="F44" s="0" t="s">
-        <x:v>148</x:v>
+        <x:v>145</x:v>
       </x:c>
       <x:c r="G44" s="0" t="s">
         <x:v>13</x:v>
@@ -2476,7 +2476,7 @@
         <x:v>175</x:v>
       </x:c>
       <x:c r="F45" s="0" t="s">
-        <x:v>148</x:v>
+        <x:v>145</x:v>
       </x:c>
       <x:c r="G45" s="0" t="s">
         <x:v>161</x:v>
@@ -2499,10 +2499,10 @@
         <x:v>179</x:v>
       </x:c>
       <x:c r="F46" s="0" t="s">
-        <x:v>148</x:v>
+        <x:v>145</x:v>
       </x:c>
       <x:c r="G46" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>26</x:v>
       </x:c>
     </x:row>
     <x:row r="47" spans="1:7">
@@ -2522,7 +2522,7 @@
         <x:v>183</x:v>
       </x:c>
       <x:c r="F47" s="0" t="s">
-        <x:v>148</x:v>
+        <x:v>145</x:v>
       </x:c>
       <x:c r="G47" s="0" t="s">
         <x:v>40</x:v>
@@ -2545,7 +2545,7 @@
         <x:v>187</x:v>
       </x:c>
       <x:c r="F48" s="0" t="s">
-        <x:v>148</x:v>
+        <x:v>145</x:v>
       </x:c>
       <x:c r="G48" s="0" t="s">
         <x:v>136</x:v>
@@ -2568,10 +2568,10 @@
         <x:v>191</x:v>
       </x:c>
       <x:c r="F49" s="0" t="s">
-        <x:v>148</x:v>
+        <x:v>145</x:v>
       </x:c>
       <x:c r="G49" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>26</x:v>
       </x:c>
     </x:row>
     <x:row r="50" spans="1:7">
@@ -2591,7 +2591,7 @@
         <x:v>195</x:v>
       </x:c>
       <x:c r="F50" s="0" t="s">
-        <x:v>148</x:v>
+        <x:v>145</x:v>
       </x:c>
       <x:c r="G50" s="0" t="s">
         <x:v>196</x:v>
@@ -2614,7 +2614,7 @@
         <x:v>183</x:v>
       </x:c>
       <x:c r="F51" s="0" t="s">
-        <x:v>148</x:v>
+        <x:v>145</x:v>
       </x:c>
       <x:c r="G51" s="0" t="s">
         <x:v>40</x:v>
@@ -2637,7 +2637,7 @@
         <x:v>202</x:v>
       </x:c>
       <x:c r="F52" s="0" t="s">
-        <x:v>148</x:v>
+        <x:v>145</x:v>
       </x:c>
       <x:c r="G52" s="0" t="s">
         <x:v>70</x:v>
@@ -2660,10 +2660,10 @@
         <x:v>206</x:v>
       </x:c>
       <x:c r="F53" s="0" t="s">
-        <x:v>148</x:v>
+        <x:v>145</x:v>
       </x:c>
       <x:c r="G53" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>26</x:v>
       </x:c>
     </x:row>
     <x:row r="54" spans="1:7">
@@ -2683,7 +2683,7 @@
         <x:v>187</x:v>
       </x:c>
       <x:c r="F54" s="0" t="s">
-        <x:v>148</x:v>
+        <x:v>145</x:v>
       </x:c>
       <x:c r="G54" s="0" t="s">
         <x:v>136</x:v>
@@ -2706,7 +2706,7 @@
         <x:v>211</x:v>
       </x:c>
       <x:c r="F55" s="0" t="s">
-        <x:v>148</x:v>
+        <x:v>145</x:v>
       </x:c>
       <x:c r="G55" s="0" t="s">
         <x:v>13</x:v>
@@ -2729,10 +2729,10 @@
         <x:v>215</x:v>
       </x:c>
       <x:c r="F56" s="0" t="s">
-        <x:v>148</x:v>
+        <x:v>145</x:v>
       </x:c>
       <x:c r="G56" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>26</x:v>
       </x:c>
     </x:row>
     <x:row r="57" spans="1:7">
@@ -2752,7 +2752,7 @@
         <x:v>219</x:v>
       </x:c>
       <x:c r="F57" s="0" t="s">
-        <x:v>148</x:v>
+        <x:v>145</x:v>
       </x:c>
       <x:c r="G57" s="0" t="s">
         <x:v>40</x:v>
@@ -2775,7 +2775,7 @@
         <x:v>223</x:v>
       </x:c>
       <x:c r="F58" s="0" t="s">
-        <x:v>148</x:v>
+        <x:v>145</x:v>
       </x:c>
       <x:c r="G58" s="0" t="s">
         <x:v>121</x:v>
@@ -2798,7 +2798,7 @@
         <x:v>227</x:v>
       </x:c>
       <x:c r="F59" s="0" t="s">
-        <x:v>148</x:v>
+        <x:v>145</x:v>
       </x:c>
       <x:c r="G59" s="0" t="s">
         <x:v>13</x:v>
@@ -2821,10 +2821,10 @@
         <x:v>231</x:v>
       </x:c>
       <x:c r="F60" s="0" t="s">
-        <x:v>148</x:v>
+        <x:v>145</x:v>
       </x:c>
       <x:c r="G60" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>26</x:v>
       </x:c>
     </x:row>
     <x:row r="61" spans="1:7">
@@ -2835,7 +2835,7 @@
         <x:v>233</x:v>
       </x:c>
       <x:c r="C61" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>45</x:v>
       </x:c>
       <x:c r="D61" s="0" t="s">
         <x:v>10</x:v>
@@ -2844,10 +2844,10 @@
         <x:v>24</x:v>
       </x:c>
       <x:c r="F61" s="0" t="s">
-        <x:v>148</x:v>
+        <x:v>145</x:v>
       </x:c>
       <x:c r="G61" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>26</x:v>
       </x:c>
     </x:row>
     <x:row r="62" spans="1:7">
@@ -2867,7 +2867,7 @@
         <x:v>237</x:v>
       </x:c>
       <x:c r="F62" s="0" t="s">
-        <x:v>148</x:v>
+        <x:v>145</x:v>
       </x:c>
       <x:c r="G62" s="0" t="s">
         <x:v>13</x:v>
@@ -2890,7 +2890,7 @@
         <x:v>130</x:v>
       </x:c>
       <x:c r="F63" s="0" t="s">
-        <x:v>148</x:v>
+        <x:v>145</x:v>
       </x:c>
       <x:c r="G63" s="0" t="s">
         <x:v>13</x:v>
@@ -2913,7 +2913,7 @@
         <x:v>237</x:v>
       </x:c>
       <x:c r="F64" s="0" t="s">
-        <x:v>148</x:v>
+        <x:v>145</x:v>
       </x:c>
       <x:c r="G64" s="0" t="s">
         <x:v>13</x:v>
@@ -2936,7 +2936,7 @@
         <x:v>171</x:v>
       </x:c>
       <x:c r="F65" s="0" t="s">
-        <x:v>148</x:v>
+        <x:v>145</x:v>
       </x:c>
       <x:c r="G65" s="0" t="s">
         <x:v>13</x:v>
@@ -2959,7 +2959,7 @@
         <x:v>237</x:v>
       </x:c>
       <x:c r="F66" s="0" t="s">
-        <x:v>148</x:v>
+        <x:v>145</x:v>
       </x:c>
       <x:c r="G66" s="0" t="s">
         <x:v>13</x:v>
@@ -2982,7 +2982,7 @@
         <x:v>247</x:v>
       </x:c>
       <x:c r="F67" s="0" t="s">
-        <x:v>148</x:v>
+        <x:v>145</x:v>
       </x:c>
       <x:c r="G67" s="0" t="s">
         <x:v>121</x:v>
@@ -3005,7 +3005,7 @@
         <x:v>251</x:v>
       </x:c>
       <x:c r="F68" s="0" t="s">
-        <x:v>148</x:v>
+        <x:v>145</x:v>
       </x:c>
       <x:c r="G68" s="0" t="s">
         <x:v>136</x:v>
@@ -3028,7 +3028,7 @@
         <x:v>255</x:v>
       </x:c>
       <x:c r="F69" s="0" t="s">
-        <x:v>148</x:v>
+        <x:v>145</x:v>
       </x:c>
       <x:c r="G69" s="0" t="s">
         <x:v>13</x:v>
@@ -3051,7 +3051,7 @@
         <x:v>130</x:v>
       </x:c>
       <x:c r="F70" s="0" t="s">
-        <x:v>148</x:v>
+        <x:v>145</x:v>
       </x:c>
       <x:c r="G70" s="0" t="s">
         <x:v>13</x:v>
@@ -3074,7 +3074,7 @@
         <x:v>237</x:v>
       </x:c>
       <x:c r="F71" s="0" t="s">
-        <x:v>148</x:v>
+        <x:v>145</x:v>
       </x:c>
       <x:c r="G71" s="0" t="s">
         <x:v>13</x:v>
@@ -3097,7 +3097,7 @@
         <x:v>262</x:v>
       </x:c>
       <x:c r="F72" s="0" t="s">
-        <x:v>148</x:v>
+        <x:v>145</x:v>
       </x:c>
       <x:c r="G72" s="0" t="s">
         <x:v>13</x:v>
@@ -3120,7 +3120,7 @@
         <x:v>266</x:v>
       </x:c>
       <x:c r="F73" s="0" t="s">
-        <x:v>148</x:v>
+        <x:v>145</x:v>
       </x:c>
       <x:c r="G73" s="0" t="s">
         <x:v>267</x:v>
@@ -3143,7 +3143,7 @@
         <x:v>271</x:v>
       </x:c>
       <x:c r="F74" s="0" t="s">
-        <x:v>148</x:v>
+        <x:v>145</x:v>
       </x:c>
       <x:c r="G74" s="0" t="s">
         <x:v>136</x:v>
@@ -3166,7 +3166,7 @@
         <x:v>275</x:v>
       </x:c>
       <x:c r="F75" s="0" t="s">
-        <x:v>148</x:v>
+        <x:v>145</x:v>
       </x:c>
       <x:c r="G75" s="0" t="s">
         <x:v>20</x:v>
@@ -3189,7 +3189,7 @@
         <x:v>279</x:v>
       </x:c>
       <x:c r="F76" s="0" t="s">
-        <x:v>148</x:v>
+        <x:v>145</x:v>
       </x:c>
       <x:c r="G76" s="0" t="s">
         <x:v>280</x:v>
@@ -3212,7 +3212,7 @@
         <x:v>284</x:v>
       </x:c>
       <x:c r="F77" s="0" t="s">
-        <x:v>148</x:v>
+        <x:v>145</x:v>
       </x:c>
       <x:c r="G77" s="0" t="s">
         <x:v>285</x:v>
@@ -3235,7 +3235,7 @@
         <x:v>237</x:v>
       </x:c>
       <x:c r="F78" s="0" t="s">
-        <x:v>148</x:v>
+        <x:v>145</x:v>
       </x:c>
       <x:c r="G78" s="0" t="s">
         <x:v>13</x:v>
@@ -3258,7 +3258,7 @@
         <x:v>284</x:v>
       </x:c>
       <x:c r="F79" s="0" t="s">
-        <x:v>148</x:v>
+        <x:v>145</x:v>
       </x:c>
       <x:c r="G79" s="0" t="s">
         <x:v>285</x:v>
@@ -3281,7 +3281,7 @@
         <x:v>292</x:v>
       </x:c>
       <x:c r="F80" s="0" t="s">
-        <x:v>148</x:v>
+        <x:v>145</x:v>
       </x:c>
       <x:c r="G80" s="0" t="s">
         <x:v>20</x:v>
@@ -3304,7 +3304,7 @@
         <x:v>284</x:v>
       </x:c>
       <x:c r="F81" s="0" t="s">
-        <x:v>148</x:v>
+        <x:v>145</x:v>
       </x:c>
       <x:c r="G81" s="0" t="s">
         <x:v>196</x:v>
@@ -3327,7 +3327,7 @@
         <x:v>297</x:v>
       </x:c>
       <x:c r="F82" s="0" t="s">
-        <x:v>148</x:v>
+        <x:v>145</x:v>
       </x:c>
       <x:c r="G82" s="0" t="s">
         <x:v>298</x:v>
@@ -3350,7 +3350,7 @@
         <x:v>284</x:v>
       </x:c>
       <x:c r="F83" s="0" t="s">
-        <x:v>148</x:v>
+        <x:v>145</x:v>
       </x:c>
       <x:c r="G83" s="0" t="s">
         <x:v>300</x:v>
@@ -3373,7 +3373,7 @@
         <x:v>304</x:v>
       </x:c>
       <x:c r="F84" s="0" t="s">
-        <x:v>148</x:v>
+        <x:v>145</x:v>
       </x:c>
       <x:c r="G84" s="0" t="s">
         <x:v>305</x:v>
@@ -3396,7 +3396,7 @@
         <x:v>309</x:v>
       </x:c>
       <x:c r="F85" s="0" t="s">
-        <x:v>148</x:v>
+        <x:v>145</x:v>
       </x:c>
       <x:c r="G85" s="0" t="s">
         <x:v>40</x:v>
@@ -3419,7 +3419,7 @@
         <x:v>255</x:v>
       </x:c>
       <x:c r="F86" s="0" t="s">
-        <x:v>148</x:v>
+        <x:v>145</x:v>
       </x:c>
       <x:c r="G86" s="0" t="s">
         <x:v>13</x:v>
@@ -3442,7 +3442,7 @@
         <x:v>304</x:v>
       </x:c>
       <x:c r="F87" s="0" t="s">
-        <x:v>148</x:v>
+        <x:v>145</x:v>
       </x:c>
       <x:c r="G87" s="0" t="s">
         <x:v>305</x:v>
@@ -3465,7 +3465,7 @@
         <x:v>317</x:v>
       </x:c>
       <x:c r="F88" s="0" t="s">
-        <x:v>148</x:v>
+        <x:v>145</x:v>
       </x:c>
       <x:c r="G88" s="0" t="s">
         <x:v>13</x:v>
@@ -3488,7 +3488,7 @@
         <x:v>321</x:v>
       </x:c>
       <x:c r="F89" s="0" t="s">
-        <x:v>148</x:v>
+        <x:v>322</x:v>
       </x:c>
       <x:c r="G89" s="0" t="s">
         <x:v>40</x:v>
@@ -3496,22 +3496,22 @@
     </x:row>
     <x:row r="90" spans="1:7">
       <x:c r="A90" s="0" t="s">
+        <x:v>323</x:v>
+      </x:c>
+      <x:c r="B90" s="0" t="s">
+        <x:v>324</x:v>
+      </x:c>
+      <x:c r="C90" s="0" t="s">
+        <x:v>325</x:v>
+      </x:c>
+      <x:c r="D90" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="E90" s="0" t="s">
+        <x:v>326</x:v>
+      </x:c>
+      <x:c r="F90" s="0" t="s">
         <x:v>322</x:v>
-      </x:c>
-      <x:c r="B90" s="0" t="s">
-        <x:v>323</x:v>
-      </x:c>
-      <x:c r="C90" s="0" t="s">
-        <x:v>324</x:v>
-      </x:c>
-      <x:c r="D90" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="E90" s="0" t="s">
-        <x:v>325</x:v>
-      </x:c>
-      <x:c r="F90" s="0" t="s">
-        <x:v>148</x:v>
       </x:c>
       <x:c r="G90" s="0" t="s">
         <x:v>13</x:v>
@@ -3519,22 +3519,22 @@
     </x:row>
     <x:row r="91" spans="1:7">
       <x:c r="A91" s="0" t="s">
-        <x:v>326</x:v>
+        <x:v>327</x:v>
       </x:c>
       <x:c r="B91" s="0" t="s">
-        <x:v>327</x:v>
+        <x:v>328</x:v>
       </x:c>
       <x:c r="C91" s="0" t="s">
-        <x:v>328</x:v>
+        <x:v>329</x:v>
       </x:c>
       <x:c r="D91" s="0" t="s">
         <x:v>10</x:v>
       </x:c>
       <x:c r="E91" s="0" t="s">
-        <x:v>329</x:v>
+        <x:v>330</x:v>
       </x:c>
       <x:c r="F91" s="0" t="s">
-        <x:v>330</x:v>
+        <x:v>322</x:v>
       </x:c>
       <x:c r="G91" s="0" t="s">
         <x:v>57</x:v>
@@ -3557,7 +3557,7 @@
         <x:v>284</x:v>
       </x:c>
       <x:c r="F92" s="0" t="s">
-        <x:v>330</x:v>
+        <x:v>322</x:v>
       </x:c>
       <x:c r="G92" s="0" t="s">
         <x:v>196</x:v>
@@ -3580,7 +3580,7 @@
         <x:v>335</x:v>
       </x:c>
       <x:c r="F93" s="0" t="s">
-        <x:v>330</x:v>
+        <x:v>322</x:v>
       </x:c>
       <x:c r="G93" s="0" t="s">
         <x:v>89</x:v>
@@ -3588,22 +3588,22 @@
     </x:row>
     <x:row r="94" spans="1:7">
       <x:c r="A94" s="0" t="s">
-        <x:v>326</x:v>
+        <x:v>327</x:v>
       </x:c>
       <x:c r="B94" s="0" t="s">
         <x:v>336</x:v>
       </x:c>
       <x:c r="C94" s="0" t="s">
-        <x:v>328</x:v>
+        <x:v>329</x:v>
       </x:c>
       <x:c r="D94" s="0" t="s">
         <x:v>10</x:v>
       </x:c>
       <x:c r="E94" s="0" t="s">
-        <x:v>329</x:v>
+        <x:v>330</x:v>
       </x:c>
       <x:c r="F94" s="0" t="s">
-        <x:v>330</x:v>
+        <x:v>322</x:v>
       </x:c>
       <x:c r="G94" s="0" t="s">
         <x:v>337</x:v>
@@ -3626,7 +3626,7 @@
         <x:v>341</x:v>
       </x:c>
       <x:c r="F95" s="0" t="s">
-        <x:v>330</x:v>
+        <x:v>322</x:v>
       </x:c>
       <x:c r="G95" s="0" t="s">
         <x:v>342</x:v>
@@ -3634,22 +3634,22 @@
     </x:row>
     <x:row r="96" spans="1:7">
       <x:c r="A96" s="0" t="s">
-        <x:v>326</x:v>
+        <x:v>327</x:v>
       </x:c>
       <x:c r="B96" s="0" t="s">
         <x:v>343</x:v>
       </x:c>
       <x:c r="C96" s="0" t="s">
-        <x:v>328</x:v>
+        <x:v>329</x:v>
       </x:c>
       <x:c r="D96" s="0" t="s">
         <x:v>10</x:v>
       </x:c>
       <x:c r="E96" s="0" t="s">
-        <x:v>329</x:v>
+        <x:v>330</x:v>
       </x:c>
       <x:c r="F96" s="0" t="s">
-        <x:v>330</x:v>
+        <x:v>322</x:v>
       </x:c>
       <x:c r="G96" s="0" t="s">
         <x:v>280</x:v>
@@ -3672,7 +3672,7 @@
         <x:v>347</x:v>
       </x:c>
       <x:c r="F97" s="0" t="s">
-        <x:v>330</x:v>
+        <x:v>322</x:v>
       </x:c>
       <x:c r="G97" s="0" t="s">
         <x:v>280</x:v>
@@ -3695,7 +3695,7 @@
         <x:v>304</x:v>
       </x:c>
       <x:c r="F98" s="0" t="s">
-        <x:v>330</x:v>
+        <x:v>322</x:v>
       </x:c>
       <x:c r="G98" s="0" t="s">
         <x:v>305</x:v>
@@ -3718,7 +3718,7 @@
         <x:v>74</x:v>
       </x:c>
       <x:c r="F99" s="0" t="s">
-        <x:v>330</x:v>
+        <x:v>322</x:v>
       </x:c>
       <x:c r="G99" s="0" t="s">
         <x:v>351</x:v>
@@ -3741,7 +3741,7 @@
         <x:v>304</x:v>
       </x:c>
       <x:c r="F100" s="0" t="s">
-        <x:v>330</x:v>
+        <x:v>322</x:v>
       </x:c>
       <x:c r="G100" s="0" t="s">
         <x:v>305</x:v>
@@ -3764,10 +3764,10 @@
         <x:v>356</x:v>
       </x:c>
       <x:c r="F101" s="0" t="s">
-        <x:v>330</x:v>
+        <x:v>322</x:v>
       </x:c>
       <x:c r="G101" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>26</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>